<commit_message>
Restructured main.py same logic
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -613,7 +613,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -686,10 +686,10 @@
         <v>12</v>
       </c>
       <c r="Z2" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="AA2" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="AB2" t="n">
         <v>12</v>

</xml_diff>

<commit_message>
All data is read/ still need price per unit(len/quan) & type )
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -619,7 +619,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>nerreg</t>
+          <t>n</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -736,13 +736,13 @@
         <v>952</v>
       </c>
       <c r="O3" t="n">
-        <v/>
+        <v>1024.8</v>
       </c>
       <c r="P3" t="n">
-        <v/>
+        <v>559.8</v>
       </c>
       <c r="Q3" t="n">
-        <v/>
+        <v>194.4</v>
       </c>
       <c r="R3" t="n">
         <v>36</v>

</xml_diff>

<commit_message>
Unit Pricing Incorporated (Len+Units)
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -433,18 +433,18 @@
     <col width="14" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="9" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
     <col width="17" customWidth="1" min="14" max="14"/>
     <col width="16" customWidth="1" min="15" max="15"/>
     <col width="18" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="21" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
-    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="19" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
     <col width="29" customWidth="1" min="21" max="21"/>
     <col width="32" customWidth="1" min="22" max="22"/>
     <col width="33" customWidth="1" min="23" max="23"/>
-    <col width="13" customWidth="1" min="24" max="24"/>
+    <col width="19" customWidth="1" min="24" max="24"/>
     <col width="13" customWidth="1" min="25" max="25"/>
     <col width="18" customWidth="1" min="26" max="26"/>
     <col width="15" customWidth="1" min="27" max="27"/>
@@ -619,7 +619,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>n</t>
+          <t>work</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -727,61 +727,61 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
-        <v>90720</v>
+        <v>181.44</v>
       </c>
       <c r="M3" t="n">
-        <v>129.6</v>
+        <v>6.48</v>
       </c>
       <c r="N3" t="n">
-        <v>952</v>
+        <v>19.04</v>
       </c>
       <c r="O3" t="n">
-        <v>1024.8</v>
+        <v>10.248</v>
       </c>
       <c r="P3" t="n">
-        <v>559.8</v>
+        <v>5.598</v>
       </c>
       <c r="Q3" t="n">
-        <v>194.4</v>
+        <v>1.944</v>
       </c>
       <c r="R3" t="n">
         <v>36</v>
       </c>
       <c r="S3" t="n">
-        <v>461.7</v>
+        <v>9.234000000000002</v>
       </c>
       <c r="T3" t="n">
-        <v>615.6</v>
+        <v>12.312</v>
       </c>
       <c r="U3" t="n">
-        <v>588</v>
+        <v>11.76</v>
       </c>
       <c r="V3" t="n">
-        <v>340.2</v>
+        <v>6.804</v>
       </c>
       <c r="W3" t="n">
-        <v>762</v>
+        <v>15.24</v>
       </c>
       <c r="X3" t="n">
-        <v>6704</v>
+        <v>279.3333333333333</v>
       </c>
       <c r="Y3" t="n">
-        <v>5028</v>
+        <v>209.5</v>
       </c>
       <c r="Z3" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>11928</v>
+        <v>497</v>
       </c>
       <c r="AB3" t="n">
-        <v>6324</v>
+        <v>263.5</v>
       </c>
       <c r="AC3" t="n">
-        <v>5328</v>
+        <v>222</v>
       </c>
       <c r="AD3" t="n">
-        <v>3168</v>
+        <v>132</v>
       </c>
       <c r="AE3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Added Row of Part Numbers
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,178 +612,286 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>YES 45TU FRONT SET(OG)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" t="n">
-        <v>144</v>
-      </c>
-      <c r="G2" t="n">
-        <v>96</v>
-      </c>
-      <c r="H2" t="n">
-        <v>96</v>
-      </c>
-      <c r="I2" t="n">
-        <v>96</v>
-      </c>
-      <c r="J2" t="n">
-        <v>40</v>
-      </c>
-      <c r="K2" t="n">
-        <v>40</v>
-      </c>
-      <c r="L2" t="n">
-        <v>224</v>
-      </c>
-      <c r="M2" t="n">
-        <v>2</v>
-      </c>
-      <c r="N2" t="n">
-        <v>8</v>
-      </c>
-      <c r="O2" t="n">
-        <v>56</v>
-      </c>
-      <c r="P2" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>4</v>
-      </c>
-      <c r="R2" t="n">
-        <v>8</v>
-      </c>
-      <c r="S2" t="n">
-        <v>6</v>
-      </c>
-      <c r="T2" t="n">
-        <v>8</v>
-      </c>
-      <c r="U2" t="n">
-        <v>4</v>
-      </c>
-      <c r="V2" t="n">
-        <v>6</v>
-      </c>
-      <c r="W2" t="n">
-        <v>8</v>
-      </c>
-      <c r="X2" t="n">
-        <v>16</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>12</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>24</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>24</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>12</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>12</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>12</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>18</v>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>E2-0052</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>E1-0199</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>E2-0047</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>PC-1220</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>PM-1006-SS</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>UA-1212</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>E1-2530</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>E2-0166</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>E2-0177</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>E2-0545</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>E2-0154</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>E2-0611</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>BE9-2512</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>BE9-2511</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>BE9-2515</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>BE9-2514</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>BE9-2578</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>YES 45TU FRONT SET(OG)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>144</v>
+      </c>
+      <c r="G3" t="n">
+        <v>96</v>
+      </c>
+      <c r="H3" t="n">
+        <v>96</v>
+      </c>
+      <c r="I3" t="n">
+        <v>96</v>
+      </c>
+      <c r="J3" t="n">
+        <v>40</v>
+      </c>
+      <c r="K3" t="n">
+        <v>40</v>
+      </c>
+      <c r="L3" t="n">
+        <v>224</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" t="n">
+        <v>8</v>
+      </c>
+      <c r="O3" t="n">
+        <v>56</v>
+      </c>
+      <c r="P3" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R3" t="n">
+        <v>8</v>
+      </c>
+      <c r="S3" t="n">
+        <v>6</v>
+      </c>
+      <c r="T3" t="n">
+        <v>8</v>
+      </c>
+      <c r="U3" t="n">
+        <v>4</v>
+      </c>
+      <c r="V3" t="n">
+        <v>6</v>
+      </c>
+      <c r="W3" t="n">
+        <v>8</v>
+      </c>
+      <c r="X3" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Total Cost ($)</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
         <v>181.44</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M4" t="n">
         <v>6.48</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N4" t="n">
         <v>19.04</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O4" t="n">
         <v>10.248</v>
       </c>
-      <c r="P3" t="n">
+      <c r="P4" t="n">
         <v>5.598</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q4" t="n">
         <v>1.944</v>
       </c>
-      <c r="R3" t="n">
+      <c r="R4" t="n">
         <v>36</v>
       </c>
-      <c r="S3" t="n">
+      <c r="S4" t="n">
         <v>9.234000000000002</v>
       </c>
-      <c r="T3" t="n">
+      <c r="T4" t="n">
         <v>12.312</v>
       </c>
-      <c r="U3" t="n">
+      <c r="U4" t="n">
         <v>11.76</v>
       </c>
-      <c r="V3" t="n">
+      <c r="V4" t="n">
         <v>6.804</v>
       </c>
-      <c r="W3" t="n">
+      <c r="W4" t="n">
         <v>15.24</v>
       </c>
-      <c r="X3" t="n">
+      <c r="X4" t="n">
         <v>279.3333333333333</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="Y4" t="n">
         <v>209.5</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="Z4" t="n">
         <v>0</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AA4" t="n">
         <v>497</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AB4" t="n">
         <v>263.5</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AC4" t="n">
         <v>222</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AD4" t="n">
         <v>132</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AE4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Finish Multiplier Integrated with GUI
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -444,13 +444,13 @@
     <col width="29" customWidth="1" min="21" max="21"/>
     <col width="32" customWidth="1" min="22" max="22"/>
     <col width="33" customWidth="1" min="23" max="23"/>
-    <col width="19" customWidth="1" min="24" max="24"/>
+    <col width="20" customWidth="1" min="24" max="24"/>
     <col width="13" customWidth="1" min="25" max="25"/>
     <col width="18" customWidth="1" min="26" max="26"/>
     <col width="15" customWidth="1" min="27" max="27"/>
     <col width="20" customWidth="1" min="28" max="28"/>
     <col width="13" customWidth="1" min="29" max="29"/>
-    <col width="19" customWidth="1" min="30" max="30"/>
+    <col width="20" customWidth="1" min="30" max="30"/>
     <col width="20" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
@@ -718,6 +718,11 @@
           <t>BE9-2578</t>
         </is>
       </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -871,25 +876,25 @@
         <v>15.24</v>
       </c>
       <c r="X4" t="n">
-        <v>279.3333333333333</v>
+        <v>27933389.2</v>
       </c>
       <c r="Y4" t="n">
-        <v>209.5</v>
+        <v>20950041.9</v>
       </c>
       <c r="Z4" t="n">
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>497</v>
+        <v>49700099.4</v>
       </c>
       <c r="AB4" t="n">
-        <v>263.5</v>
+        <v>26350052.7</v>
       </c>
       <c r="AC4" t="n">
-        <v>222</v>
+        <v>22200044.4</v>
       </c>
       <c r="AD4" t="n">
-        <v>132</v>
+        <v>13200026.4</v>
       </c>
       <c r="AE4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
took away ft vs pcs quantity unit
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -687,92 +687,92 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>224.0 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>8 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>56 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>12 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>4 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>8 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>6 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>8 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>4 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>6 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>8 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>12.0 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>24.0 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>24.0 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>12.0 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>12.0 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>12.0 pcs</t>
+          <t>18 pcs</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>$181.44</t>
+          <t>$217.73</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -862,7 +862,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>$209.50</t>
+          <t>$251.40</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -872,22 +872,22 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>$497.00</t>
+          <t>$596.40</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>$263.50</t>
+          <t>$316.20</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>$222.00</t>
+          <t>$266.40</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>$132.00</t>
+          <t>$158.40</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>$1640.10</t>
+          <t>$1941.19</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Profiles and Accessories heading In Excel
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,26 +424,20 @@
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="24" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="31" customWidth="1" min="5" max="5"/>
-    <col width="27" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
-    <col width="76" customWidth="1" min="8" max="8"/>
-    <col width="78" customWidth="1" min="9" max="9"/>
-    <col width="68" customWidth="1" min="10" max="10"/>
-    <col width="60" customWidth="1" min="11" max="11"/>
-    <col width="53" customWidth="1" min="12" max="12"/>
-    <col width="24" customWidth="1" min="13" max="13"/>
-    <col width="32" customWidth="1" min="14" max="14"/>
-    <col width="59" customWidth="1" min="15" max="15"/>
-    <col width="43" customWidth="1" min="16" max="16"/>
-    <col width="33" customWidth="1" min="17" max="17"/>
-    <col width="14" customWidth="1" min="18" max="18"/>
-    <col width="41" customWidth="1" min="19" max="19"/>
-    <col width="34" customWidth="1" min="20" max="20"/>
-    <col width="10" customWidth="1" min="21" max="21"/>
-    <col width="23" customWidth="1" min="22" max="22"/>
-    <col width="13" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="33" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="7" max="7"/>
+    <col width="41" customWidth="1" min="8" max="8"/>
+    <col width="76" customWidth="1" min="9" max="9"/>
+    <col width="78" customWidth="1" min="10" max="10"/>
+    <col width="68" customWidth="1" min="11" max="11"/>
+    <col width="60" customWidth="1" min="12" max="12"/>
+    <col width="53" customWidth="1" min="13" max="13"/>
+    <col width="24" customWidth="1" min="14" max="14"/>
+    <col width="32" customWidth="1" min="15" max="15"/>
+    <col width="59" customWidth="1" min="16" max="16"/>
+    <col width="43" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -457,97 +451,37 @@
           <t>YES 45TU FRONT SET(OG)</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>OUTPUT</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Glazing Gasket For 1” Glazing</t>
+          <t>PROFILES</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>End Dam For Sill Flashing</t>
+          <t>Sill/Jamb Screw Spline Assembly</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Water Deflector</t>
+          <t>Flush Filler</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>#12 x 1-1/4” PHSMS Type AB, Zinc Plated Steel, For Screw Spline Attachment</t>
+          <t>Two Piece Mullion Screw Spline Assembly</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>#10-24 x 3/8” PHMS, Stainless Steel, For Attachment of Sill to Sill Flashing</t>
+          <t>Horizontal Screw Spline Assembly</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>#12 x 3/4” UFHSMS Type A, Zinc Plated Steel For End Dam Attachment</t>
+          <t>Head</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
-        <is>
-          <t>Setting Block Chair Use with E2-0177 Setting Block at Sill</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Side Block For Intermediate Vertical Shallow Pocket</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Setting Block For Sill</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>1-1/8” “W” Side Block For Jamb</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>1/2” “W” Side Block For Intermediate Vertical Deep Pocket</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Setting Block For Intermediate Horizontal</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Sill/Jamb Screw Spline Assembly</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Flush Filler</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Two Piece Mullion Screw Spline Assembly</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Horizontal Screw Spline Assembly</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Head</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
         <is>
           <t>Thermal Sill Flashing</t>
         </is>
@@ -564,97 +498,37 @@
           <t>1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Part Number</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>E2-0052</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>E1-0199</t>
+          <t>BE9-2513</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>E2-0047</t>
+          <t>E9-2512</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>PC-1220</t>
+          <t>BE9-2511</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>PM-1006-SS</t>
+          <t>BE9-2515</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>UA-1212</t>
+          <t>BE9-2514</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
-        <is>
-          <t>E1-2530</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>E2-0166</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>E2-0177</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>E2-0545</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>E2-0154</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>E2-0611</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>BE9-2513</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>E9-2512</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>BE9-2511</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>BE9-2515</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>BE9-2514</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
         <is>
           <t>BE9-2578</t>
         </is>
@@ -669,104 +543,39 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>224.0 ft</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>12.0 ft</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>8 pcs</t>
+          <t>24.0 ft</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>56 pcs</t>
+          <t>24.0 ft</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>12 pcs</t>
+          <t>12.0 ft</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>4 pcs</t>
+          <t>12.0 ft</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>8 pcs</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>6 pcs</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>8 pcs</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>4 pcs</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>6 pcs</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>8 pcs</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
           <t>12.0 ft</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>24.0 ft</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>24.0 ft</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>12.0 ft</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>12.0 ft</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>12.0 ft</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>GRAND TOTAL</t>
         </is>
       </c>
     </row>
@@ -779,104 +588,39 @@
       <c r="B4" t="n">
         <v>4</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>$181.44</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$6.48</t>
+          <t>$209.50</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>$19.04</t>
+          <t>$150.00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>$10.25</t>
+          <t>$497.00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>$5.60</t>
+          <t>$263.50</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>$1.94</t>
+          <t>$222.00</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>$36.00</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>$9.23</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>$12.31</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>$11.76</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>$6.80</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>$15.24</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>$209.50</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>$150.00</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>$497.00</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>$263.50</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>$222.00</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
           <t>$132.00</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>$1790.10</t>
         </is>
       </c>
     </row>
@@ -909,6 +653,71 @@
       <c r="B7" t="n">
         <v>96</v>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ACCESSORIES</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Glazing Gasket For 1” Glazing</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>End Dam For Sill Flashing</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Water Deflector</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>#12 x 1-1/4” PHSMS Type AB, Zinc Plated Steel, For Screw Spline Attachment</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>#10-24 x 3/8” PHMS, Stainless Steel, For Attachment of Sill to Sill Flashing</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>#12 x 3/4” UFHSMS Type A, Zinc Plated Steel For End Dam Attachment</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Setting Block Chair Use with E2-0177 Setting Block at Sill</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Side Block For Intermediate Vertical Shallow Pocket</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Setting Block For Sill</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>1-1/8” “W” Side Block For Jamb</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>1/2” “W” Side Block For Intermediate Vertical Deep Pocket</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Setting Block For Intermediate Horizontal</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -919,6 +728,71 @@
       <c r="B8" t="n">
         <v>96</v>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>E2-0052</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>E1-0199</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>E2-0047</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>PC-1220</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>PM-1006-SS</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>UA-1212</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>E1-2530</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>E2-0166</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>E2-0177</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>E2-0545</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>E2-0154</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>E2-0611</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -929,6 +803,71 @@
       <c r="B9" t="n">
         <v>96</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>224.0 ft</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>56 pcs</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>12 pcs</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>4 pcs</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>6 pcs</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>4 pcs</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>6 pcs</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -939,6 +878,71 @@
       <c r="B10" t="n">
         <v>40</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>$181.44</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>$6.48</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>$19.04</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>$10.25</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>$5.60</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>$1.94</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>$36.00</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>$9.23</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>$12.31</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>$11.76</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>$6.80</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>$15.24</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -948,6 +952,21 @@
       </c>
       <c r="B11" t="n">
         <v>40</v>
+      </c>
+    </row>
+    <row r="12"/>
+    <row r="13">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>GRAND TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>$1790.10</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Duplciate Part Numbers
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -427,8 +427,8 @@
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="33" customWidth="1" min="6" max="6"/>
-    <col width="27" customWidth="1" min="7" max="7"/>
-    <col width="41" customWidth="1" min="8" max="8"/>
+    <col width="33" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="8" max="8"/>
     <col width="76" customWidth="1" min="9" max="9"/>
     <col width="78" customWidth="1" min="10" max="10"/>
     <col width="68" customWidth="1" min="11" max="11"/>
@@ -463,25 +463,30 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>Sill/Jamb Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>Flush Filler</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Two Piece Mullion Screw Spline Assembly</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Horizontal Screw Spline Assembly</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Head</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Thermal Sill Flashing</t>
         </is>
@@ -510,25 +515,30 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>E9-2512</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>BE9-2511</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>BE9-2515</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>BE9-2514</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>BE9-2578</t>
         </is>
@@ -550,30 +560,35 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>16.0 ft</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>12.0 ft</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>24.0 ft</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>24.0 ft</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>12.0 ft</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>12.0 ft</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>12.0 ft</t>
         </is>
@@ -595,32 +610,37 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$209.50</t>
+          <t>$335.20</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>$150.00</t>
+          <t>$251.40</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>$497.00</t>
+          <t>$180.00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>$263.50</t>
+          <t>$596.40</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>$222.00</t>
+          <t>$316.20</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>$132.00</t>
+          <t>$266.40</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>$158.40</t>
         </is>
       </c>
     </row>
@@ -965,7 +985,7 @@
     <row r="14">
       <c r="E14" t="inlineStr">
         <is>
-          <t>$1790.10</t>
+          <t>$2420.10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Glass Stop Calculations
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -491,6 +491,11 @@
           <t>Thermal Sill Flashing</t>
         </is>
       </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Glass Stop (Use with BE9-2514, BE9-2515, BE9-2517)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -543,6 +548,11 @@
           <t>BE9-2578</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>E9-2519</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -593,6 +603,11 @@
           <t>12.0 ft</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>24.0 ft</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -610,37 +625,42 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$335.20</t>
+          <t>$279.33</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>$251.40</t>
+          <t>$209.50</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>$180.00</t>
+          <t>$150.00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>$596.40</t>
+          <t>$497.00</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>$316.20</t>
+          <t>$263.50</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>$266.40</t>
+          <t>$222.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>$158.40</t>
+          <t>$132.00</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>$85.05</t>
         </is>
       </c>
     </row>
@@ -985,7 +1005,7 @@
     <row r="14">
       <c r="E14" t="inlineStr">
         <is>
-          <t>$2420.10</t>
+          <t>$2154.48</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Manual Inputs w/out Part #s
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,8 +423,8 @@
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="24" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="6" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="33" customWidth="1" min="6" max="6"/>
     <col width="33" customWidth="1" min="7" max="7"/>
@@ -998,14 +998,64 @@
     <row r="13">
       <c r="E13" t="inlineStr">
         <is>
-          <t>GRAND TOTAL</t>
+          <t>GLASS</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Total Glass1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="E14" t="inlineStr">
         <is>
-          <t>$2154.48</t>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>83.75 units</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>$83.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>GRAND TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>$2238.23</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added fabrication joints & labor
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Total Glass1</t>
+          <t>Glass Area</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>83.75 units</t>
+          <t>83.75 sqft</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>$83.75</t>
+          <t>$879.38</t>
         </is>
       </c>
     </row>
@@ -1048,14 +1048,64 @@
     <row r="19">
       <c r="E19" t="inlineStr">
         <is>
-          <t>GRAND TOTAL</t>
+          <t>FABRICATION</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Joints Fabrication Labor</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="E20" t="inlineStr">
         <is>
-          <t>$2238.23</t>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>18 joints</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>$270.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>GRAND TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>$3303.86</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added a delete type
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,17 +421,743 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="2" customWidth="1" min="1" max="1"/>
-    <col width="2" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
     <col width="2" customWidth="1" min="3" max="3"/>
     <col width="2" customWidth="1" min="4" max="4"/>
-    <col width="2" customWidth="1" min="5" max="5"/>
-    <col width="2" customWidth="1" min="6" max="6"/>
-    <col width="2" customWidth="1" min="7" max="7"/>
-    <col width="2" customWidth="1" min="8" max="8"/>
+    <col width="78" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>System Input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>YES 45TU FRONT SET(OG)</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>PROFILES</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Elevation Type</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Total Count</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Sill/Jamb Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.16666666666666666 ft</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>$2.91</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t># Bays Wide</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sill/Jamb Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.08333333333333333 ft</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>$1.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t># Bays Tall</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Flush Filler</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>E9-2512</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.0 ft</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>$0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Opening Width</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Two Piece Mullion Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>BE9-2511</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.0 ft</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>$0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Opening Height</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Horizontal Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BE9-2515</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.08333333333333333 ft</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>$1.83</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sq Ft per Type</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Head</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BE9-2514</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.08333333333333333 ft</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>$1.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Total Sq Ft</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Thermal Sill Flashing</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>BE9-2578</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.08333333333333333 ft</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>$0.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Perimeter Ft</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Glass Stop (Use with BE9-2514, BE9-2515, BE9-2517)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>E9-2519</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.08333333333333333 ft</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>$0.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Total Perimeter Ft</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ACCESSORIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Glazing Gasket For 1” Glazing</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>E2-0052</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.6666666666666666 ft</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>$0.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>End Dam For Sill Flashing</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>E1-0199</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>$6.48</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Water Deflector</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>E2-0047</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>$4.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>#12 x 1-1/4” PHSMS Type AB, Zinc Plated Steel, For Screw Spline Attachment</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>PC-1220</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>$1.46</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>#10-24 x 3/8” PHMS, Stainless Steel, For Attachment of Sill to Sill Flashing</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>PM-1006-SS</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>3 pcs</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>$1.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>#12 x 3/4” UFHSMS Type A, Zinc Plated Steel For End Dam Attachment</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>UA-1212</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>4 pcs</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>$1.94</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Setting Block Chair Use with E2-0177 Setting Block at Sill</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>E1-2530</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>$9.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Side Block For Intermediate Vertical Shallow Pocket</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>E2-0166</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0 pcs</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>$0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Setting Block For Sill</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>E2-0177</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>$3.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1-1/8” “W” Side Block For Jamb</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>E2-0545</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>$5.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>1/2” “W” Side Block For Intermediate Vertical Deep Pocket</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>E2-0154</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0 pcs</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>$0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Setting Block For Intermediate Horizontal</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>E2-0611</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>$3.81</t>
+        </is>
+      </c>
+    </row>
+    <row r="26"/>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>GLASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Glass Area</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0.0625 sqft</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>$0.66</t>
+        </is>
+      </c>
+    </row>
+    <row r="30"/>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>FABRICATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Joints Fabrication Labor</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>4 joints</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>$60.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36">
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>SYSTEM TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>$107.96</t>
+        </is>
+      </c>
+    </row>
+    <row r="38"/>
+    <row r="39">
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>RUNNING GRAND TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>$107.96</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a None Option For Door
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Report" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1079,7 +1079,7 @@
     <row r="31">
       <c r="E31" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>FABRICATION</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
     <row r="33">
       <c r="E33" t="inlineStr">
         <is>
-          <t>Door size exceeds total glass area</t>
+          <t>Joints Fabrication Labor</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1118,93 +1118,40 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0 sqft</t>
+          <t>4 joints</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$60.00</t>
         </is>
       </c>
     </row>
     <row r="34"/>
     <row r="35">
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>FABRICATION</t>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>SYSTEM TOTAL</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Price</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Joints Fabrication Labor</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>4 joints</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>$60.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40">
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>SYSTEM TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="H41" t="inlineStr">
-        <is>
           <t>$107.96</t>
         </is>
       </c>
     </row>
-    <row r="42"/>
-    <row r="43">
-      <c r="H43" t="inlineStr">
+    <row r="37"/>
+    <row r="38">
+      <c r="H38" t="inlineStr">
         <is>
           <t>RUNNING GRAND TOTAL</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="H44" t="inlineStr">
+    <row r="39">
+      <c r="H39" t="inlineStr">
         <is>
           <t>$107.96</t>
         </is>

</xml_diff>

<commit_message>
Rought Draft of Summary Sheet
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -16,14 +16,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_-"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +51,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,9 +428,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
-    <col width="2" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="2" customWidth="1" min="4" max="4"/>
     <col width="78" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
@@ -431,179 +438,78 @@
     <col width="21" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>System Input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>YES 45TU FRONT SET(OG)</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>PROFILES</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Elevation Type</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Total Count</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Sill/Jamb Screw Spline Assembly</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>BE9-2513</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0.16666666666666666 ft</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>$2.91</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t># Bays Wide</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Sill/Jamb Screw Spline Assembly</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>BE9-2513</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0.08333333333333333 ft</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>$1.45</t>
-        </is>
-      </c>
-    </row>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t># Bays Tall</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
+          <t>System Input</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>YES 45TU FRONT SET(OG)</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Flush Filler</t>
+          <t>Sill/Jamb Screw Spline Assembly</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>E9-2512</t>
+          <t>BE9-2513</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.0 ft</t>
+          <t>0.16666666666666666 ft</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$2.91</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Opening Width</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
+          <t>Elevation Type</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Two Piece Mullion Screw Spline Assembly</t>
+          <t>Sill/Jamb Screw Spline Assembly</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BE9-2511</t>
+          <t>BE9-2513</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.0 ft</t>
+          <t>0.08333333333333333 ft</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$1.45</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Opening Height</t>
+          <t>Total Count</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -611,72 +517,72 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Horizontal Screw Spline Assembly</t>
+          <t>Flush Filler</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>BE9-2515</t>
+          <t>E9-2512</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.08333333333333333 ft</t>
+          <t>0.0 ft</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$1.83</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sq Ft per Type</t>
+          <t># Bays Wide</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.006944444444444444</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Head</t>
+          <t>Two Piece Mullion Screw Spline Assembly</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>BE9-2514</t>
+          <t>BE9-2511</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.08333333333333333 ft</t>
+          <t>0.0 ft</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>$1.54</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Total Sq Ft</t>
+          <t># Bays Tall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.006944444444444444</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Thermal Sill Flashing</t>
+          <t>Horizontal Screw Spline Assembly</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BE9-2578</t>
+          <t>BE9-2515</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -686,27 +592,27 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>$0.92</t>
+          <t>$1.83</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Perimeter Ft</t>
+          <t>Opening Width</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Glass Stop (Use with BE9-2514, BE9-2515, BE9-2517)</t>
+          <t>Head</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>E9-2519</t>
+          <t>BE9-2514</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -716,72 +622,119 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>$0.30</t>
+          <t>$1.54</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Opening Height</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Thermal Sill Flashing</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>BE9-2578</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.08333333333333333 ft</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>$0.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sq Ft per Type</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Glass Stop (Use with BE9-2514, BE9-2515, BE9-2517)</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>E9-2519</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.08333333333333333 ft</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>$0.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Total Sq Ft</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Perimeter Ft</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Glazing Gasket For 1” Glazing</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>E2-0052</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.6666666666666666 ft</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>$0.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Total Perimeter Ft</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B15" t="n">
         <v>0.3333333333333333</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>ACCESSORIES</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Glazing Gasket For 1” Glazing</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>E2-0052</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>0.6666666666666666 ft</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>$0.54</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
       <c r="E15" t="inlineStr">
         <is>
           <t>End Dam For Sill Flashing</t>
@@ -1027,7 +980,22 @@
     <row r="27">
       <c r="E27" t="inlineStr">
         <is>
-          <t>GLASS</t>
+          <t>Glass Area</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0.0625 sqft</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>$0.66</t>
         </is>
       </c>
     </row>
@@ -1056,7 +1024,7 @@
     <row r="29">
       <c r="E29" t="inlineStr">
         <is>
-          <t>Glass Area</t>
+          <t>Joints Fabrication Labor</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1066,94 +1034,56 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0.0625 sqft</t>
+          <t>4 joints</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>$0.66</t>
-        </is>
-      </c>
-    </row>
-    <row r="30"/>
+          <t>$60.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
     <row r="31">
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>FABRICATION</t>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>SYSTEM TOTAL</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Price</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Joints Fabrication Labor</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>4 joints</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>$60.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="34"/>
-    <row r="35">
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>SYSTEM TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="H36" t="inlineStr">
-        <is>
           <t>$107.96</t>
         </is>
       </c>
     </row>
-    <row r="37"/>
-    <row r="38">
-      <c r="H38" t="inlineStr">
+    <row r="33"/>
+    <row r="34">
+      <c r="H34" t="inlineStr">
         <is>
           <t>RUNNING GRAND TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>$107.96</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Optimal Code for Excel
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H163"/>
+  <dimension ref="A1:H160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="36" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="2" customWidth="1" min="4" max="4"/>
     <col width="78" customWidth="1" min="5" max="5"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1111</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>111111</t>
+          <t>111</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>1111</t>
         </is>
       </c>
       <c r="E68" s="1" t="inlineStr">
@@ -1836,7 +1836,7 @@
         </is>
       </c>
       <c r="H69" s="2" t="n">
-        <v>3.200694444444444</v>
+        <v>2.909722222222222</v>
       </c>
     </row>
     <row r="70">
@@ -1864,7 +1864,7 @@
         </is>
       </c>
       <c r="H70" s="2" t="n">
-        <v>1.600347222222222</v>
+        <v>1.454861111111111</v>
       </c>
     </row>
     <row r="71">
@@ -1948,7 +1948,7 @@
         </is>
       </c>
       <c r="H73" s="2" t="n">
-        <v>2.012847222222222</v>
+        <v>1.829861111111111</v>
       </c>
     </row>
     <row r="74">
@@ -1976,7 +1976,7 @@
         </is>
       </c>
       <c r="H74" s="2" t="n">
-        <v>1.695833333333333</v>
+        <v>1.541666666666667</v>
       </c>
     </row>
     <row r="75">
@@ -2004,7 +2004,7 @@
         </is>
       </c>
       <c r="H75" s="2" t="n">
-        <v>1.008333333333333</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="76">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="H76" s="2" t="n">
-        <v>0.32484375</v>
+        <v>0.2953125</v>
       </c>
     </row>
     <row r="77">
@@ -2366,7 +2366,7 @@
     <row r="95">
       <c r="E95" s="1" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>FABRICATION</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
     <row r="97">
       <c r="E97" t="inlineStr">
         <is>
-          <t>Door size exceeds total glass area</t>
+          <t>Joints Fabrication Labor</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -2405,127 +2405,162 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>0 sqft</t>
+          <t>4 joints</t>
         </is>
       </c>
       <c r="H97" s="2" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="98">
-      <c r="E98" s="1" t="inlineStr">
-        <is>
-          <t>FABRICATION</t>
+      <c r="H98" s="1" t="inlineStr">
+        <is>
+          <t>SYSTEM TOTAL</t>
         </is>
       </c>
     </row>
     <row r="99">
-      <c r="E99" s="1" t="inlineStr">
+      <c r="H99" s="2" t="n">
+        <v>107.9598402777778</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>System Input</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>YES 45TU FRONT SET(OG)</t>
+        </is>
+      </c>
+      <c r="E100" s="1" t="inlineStr">
+        <is>
+          <t>PROFILES</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Elevation Type</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="E101" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F99" s="1" t="inlineStr">
+      <c r="F101" s="1" t="inlineStr">
         <is>
           <t>Part Number</t>
         </is>
       </c>
-      <c r="G99" s="1" t="inlineStr">
+      <c r="G101" s="1" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="H99" s="1" t="inlineStr">
+      <c r="H101" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
     </row>
-    <row r="100">
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>Joints Fabrication Labor</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>4 joints</t>
-        </is>
-      </c>
-      <c r="H100" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="H101" s="1" t="inlineStr">
-        <is>
-          <t>SYSTEM TOTAL</t>
-        </is>
-      </c>
-    </row>
     <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>Total Count</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Sill/Jamb Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>0.16666666666666666 ft</t>
+        </is>
+      </c>
       <c r="H102" s="2" t="n">
-        <v>108.8546493055556</v>
+        <v>2.909722222222222</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>System Input</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>YES 45TU FRONT SET(OG)</t>
-        </is>
-      </c>
-      <c r="E103" s="1" t="inlineStr">
-        <is>
-          <t>PROFILES</t>
-        </is>
+          <t># Bays Wide</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Sill/Jamb Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>0.08333333333333333 ft</t>
+        </is>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>1.454861111111111</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>Elevation Type</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>111111111</t>
-        </is>
-      </c>
-      <c r="E104" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F104" s="1" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="G104" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="H104" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
+          <t># Bays Tall</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Flush Filler</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>E9-2512</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>0.0 ft</t>
+        </is>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>Total Count</t>
+          <t>Opening Width</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -2533,27 +2568,27 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Sill/Jamb Screw Spline Assembly</t>
+          <t>Two Piece Mullion Screw Spline Assembly</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>BE9-2513</t>
+          <t>BE9-2511</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>0.16666666666666666 ft</t>
+          <t>0.0 ft</t>
         </is>
       </c>
       <c r="H105" s="2" t="n">
-        <v>3.200694444444444</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t># Bays Wide</t>
+          <t>Opening Height</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -2561,12 +2596,12 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Sill/Jamb Screw Spline Assembly</t>
+          <t>Horizontal Screw Spline Assembly</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>BE9-2513</t>
+          <t>BE9-2515</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -2575,82 +2610,82 @@
         </is>
       </c>
       <c r="H106" s="2" t="n">
-        <v>1.600347222222222</v>
+        <v>1.829861111111111</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t># Bays Tall</t>
+          <t>Sq Ft per Type</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>1</v>
+        <v>0.006944444444444444</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Flush Filler</t>
+          <t>Head</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>E9-2512</t>
+          <t>BE9-2514</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>0.0 ft</t>
+          <t>0.08333333333333333 ft</t>
         </is>
       </c>
       <c r="H107" s="2" t="n">
-        <v>0</v>
+        <v>1.541666666666667</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>Opening Width</t>
+          <t>Total Sq Ft</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>1</v>
+        <v>0.006944444444444444</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Two Piece Mullion Screw Spline Assembly</t>
+          <t>Thermal Sill Flashing</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>BE9-2511</t>
+          <t>BE9-2578</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>0.0 ft</t>
+          <t>0.08333333333333333 ft</t>
         </is>
       </c>
       <c r="H108" s="2" t="n">
-        <v>0</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>Opening Height</t>
+          <t>Perimeter Ft</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Horizontal Screw Spline Assembly</t>
+          <t>Glass Stop (Use with BE9-2514, BE9-2515, BE9-2517)</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>BE9-2515</t>
+          <t>E9-2519</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -2659,261 +2694,237 @@
         </is>
       </c>
       <c r="H109" s="2" t="n">
-        <v>2.012847222222222</v>
+        <v>0.2953125</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>Sq Ft per Type</t>
+          <t>Total Perimeter Ft</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.006944444444444444</v>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>Head</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>BE9-2514</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>0.08333333333333333 ft</t>
-        </is>
-      </c>
-      <c r="H110" s="2" t="n">
-        <v>1.695833333333333</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="inlineStr">
-        <is>
-          <t>Total Sq Ft</t>
-        </is>
-      </c>
-      <c r="B111" t="n">
-        <v>0.006944444444444444</v>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>Thermal Sill Flashing</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>BE9-2578</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>0.08333333333333333 ft</t>
-        </is>
-      </c>
-      <c r="H111" s="2" t="n">
-        <v>1.008333333333333</v>
+      <c r="E111" s="1" t="inlineStr">
+        <is>
+          <t>ACCESSORIES</t>
+        </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="inlineStr">
-        <is>
-          <t>Perimeter Ft</t>
-        </is>
-      </c>
-      <c r="B112" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>Glass Stop (Use with BE9-2514, BE9-2515, BE9-2517)</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>E9-2519</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>0.08333333333333333 ft</t>
-        </is>
-      </c>
-      <c r="H112" s="2" t="n">
-        <v>0.32484375</v>
+      <c r="E112" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F112" s="1" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G112" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H112" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="inlineStr">
-        <is>
-          <t>Total Perimeter Ft</t>
-        </is>
-      </c>
-      <c r="B113" t="n">
-        <v>0.3333333333333333</v>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Glazing Gasket For 1” Glazing</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>E2-0052</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>0.6666666666666666 ft</t>
+        </is>
+      </c>
+      <c r="H113" s="2" t="n">
+        <v>0.54</v>
       </c>
     </row>
     <row r="114">
-      <c r="E114" s="1" t="inlineStr">
-        <is>
-          <t>ACCESSORIES</t>
-        </is>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>End Dam For Sill Flashing</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>E1-0199</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H114" s="2" t="n">
+        <v>6.48</v>
       </c>
     </row>
     <row r="115">
-      <c r="E115" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F115" s="1" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="G115" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="H115" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Water Deflector</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>E2-0047</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H115" s="2" t="n">
+        <v>4.76</v>
       </c>
     </row>
     <row r="116">
       <c r="E116" t="inlineStr">
         <is>
-          <t>Glazing Gasket For 1” Glazing</t>
+          <t>#12 x 1-1/4” PHSMS Type AB, Zinc Plated Steel, For Screw Spline Attachment</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>E2-0052</t>
+          <t>PC-1220</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>0.6666666666666666 ft</t>
+          <t>8 pcs</t>
         </is>
       </c>
       <c r="H116" s="2" t="n">
-        <v>0.54</v>
+        <v>1.464</v>
       </c>
     </row>
     <row r="117">
       <c r="E117" t="inlineStr">
         <is>
-          <t>End Dam For Sill Flashing</t>
+          <t>#10-24 x 3/8” PHMS, Stainless Steel, For Attachment of Sill to Sill Flashing</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>E1-0199</t>
+          <t>PM-1006-SS</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>3 pcs</t>
         </is>
       </c>
       <c r="H117" s="2" t="n">
-        <v>6.48</v>
+        <v>1.3995</v>
       </c>
     </row>
     <row r="118">
       <c r="E118" t="inlineStr">
         <is>
-          <t>Water Deflector</t>
+          <t>#12 x 3/4” UFHSMS Type A, Zinc Plated Steel For End Dam Attachment</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>E2-0047</t>
+          <t>UA-1212</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>4 pcs</t>
         </is>
       </c>
       <c r="H118" s="2" t="n">
-        <v>4.76</v>
+        <v>1.944</v>
       </c>
     </row>
     <row r="119">
       <c r="E119" t="inlineStr">
         <is>
-          <t>#12 x 1-1/4” PHSMS Type AB, Zinc Plated Steel, For Screw Spline Attachment</t>
+          <t>Setting Block Chair Use with E2-0177 Setting Block at Sill</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>PC-1220</t>
+          <t>E1-2530</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>8 pcs</t>
+          <t>2 pcs</t>
         </is>
       </c>
       <c r="H119" s="2" t="n">
-        <v>1.464</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120">
       <c r="E120" t="inlineStr">
         <is>
-          <t>#10-24 x 3/8” PHMS, Stainless Steel, For Attachment of Sill to Sill Flashing</t>
+          <t>Side Block For Intermediate Vertical Shallow Pocket</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>PM-1006-SS</t>
+          <t>E2-0166</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>3 pcs</t>
+          <t>0 pcs</t>
         </is>
       </c>
       <c r="H120" s="2" t="n">
-        <v>1.3995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
       <c r="E121" t="inlineStr">
         <is>
-          <t>#12 x 3/4” UFHSMS Type A, Zinc Plated Steel For End Dam Attachment</t>
+          <t>Setting Block For Sill</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>UA-1212</t>
+          <t>E2-0177</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>4 pcs</t>
+          <t>2 pcs</t>
         </is>
       </c>
       <c r="H121" s="2" t="n">
-        <v>1.944</v>
+        <v>3.078</v>
       </c>
     </row>
     <row r="122">
       <c r="E122" t="inlineStr">
         <is>
-          <t>Setting Block Chair Use with E2-0177 Setting Block at Sill</t>
+          <t>1-1/8” “W” Side Block For Jamb</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>E1-2530</t>
+          <t>E2-0545</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -2922,18 +2933,18 @@
         </is>
       </c>
       <c r="H122" s="2" t="n">
-        <v>9</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="123">
       <c r="E123" t="inlineStr">
         <is>
-          <t>Side Block For Intermediate Vertical Shallow Pocket</t>
+          <t>1/2” “W” Side Block For Intermediate Vertical Deep Pocket</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>E2-0166</t>
+          <t>E2-0154</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -2948,12 +2959,12 @@
     <row r="124">
       <c r="E124" t="inlineStr">
         <is>
-          <t>Setting Block For Sill</t>
+          <t>Setting Block For Intermediate Horizontal</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>E2-0177</t>
+          <t>E2-0611</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -2962,73 +2973,62 @@
         </is>
       </c>
       <c r="H124" s="2" t="n">
-        <v>3.078</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="125">
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>1-1/8” “W” Side Block For Jamb</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>E2-0545</t>
-        </is>
-      </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>2 pcs</t>
-        </is>
-      </c>
-      <c r="H125" s="2" t="n">
-        <v>5.88</v>
+      <c r="E125" s="1" t="inlineStr">
+        <is>
+          <t>GLASS</t>
+        </is>
       </c>
     </row>
     <row r="126">
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>1/2” “W” Side Block For Intermediate Vertical Deep Pocket</t>
-        </is>
-      </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>E2-0154</t>
-        </is>
-      </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>0 pcs</t>
-        </is>
-      </c>
-      <c r="H126" s="2" t="n">
-        <v>0</v>
+      <c r="E126" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F126" s="1" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G126" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H126" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
       </c>
     </row>
     <row r="127">
       <c r="E127" t="inlineStr">
         <is>
-          <t>Setting Block For Intermediate Horizontal</t>
+          <t>Glass Area</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>E2-0611</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>0.0625 sqft</t>
         </is>
       </c>
       <c r="H127" s="2" t="n">
-        <v>3.81</v>
+        <v>0.65625</v>
       </c>
     </row>
     <row r="128">
       <c r="E128" s="1" t="inlineStr">
         <is>
-          <t>GLASS</t>
+          <t>DOOR</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
     <row r="130">
       <c r="E130" t="inlineStr">
         <is>
-          <t>Glass Area</t>
+          <t>Door size exceeds total glass area</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -3067,17 +3067,17 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>0.0625 sqft</t>
+          <t>0 sqft</t>
         </is>
       </c>
       <c r="H130" s="2" t="n">
-        <v>0.65625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
       <c r="E131" s="1" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>FABRICATION</t>
         </is>
       </c>
     </row>
@@ -3106,7 +3106,7 @@
     <row r="133">
       <c r="E133" t="inlineStr">
         <is>
-          <t>Door size exceeds total glass area</t>
+          <t>Joints Fabrication Labor</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -3116,198 +3116,188 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>0 sqft</t>
+          <t>4 joints</t>
         </is>
       </c>
       <c r="H133" s="2" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="134">
-      <c r="E134" s="1" t="inlineStr">
-        <is>
-          <t>FABRICATION</t>
+      <c r="H134" s="1" t="inlineStr">
+        <is>
+          <t>SYSTEM TOTAL</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="E135" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F135" s="1" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="G135" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="H135" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
+      <c r="H135" s="2" t="n">
+        <v>107.9598402777778</v>
       </c>
     </row>
     <row r="136">
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>Joints Fabrication Labor</t>
-        </is>
-      </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>4 joints</t>
-        </is>
-      </c>
-      <c r="H136" s="2" t="n">
-        <v>60</v>
+      <c r="H136" s="1" t="inlineStr">
+        <is>
+          <t>RUNNING GRAND TOTAL</t>
+        </is>
       </c>
     </row>
     <row r="137">
-      <c r="H137" s="1" t="inlineStr">
-        <is>
-          <t>SYSTEM TOTAL</t>
-        </is>
+      <c r="H137" s="2" t="n">
+        <v>431.8393611111112</v>
       </c>
     </row>
     <row r="138">
-      <c r="H138" s="2" t="n">
-        <v>108.8546493055556</v>
+      <c r="A138" s="1" t="inlineStr">
+        <is>
+          <t>Part Number / Description</t>
+        </is>
+      </c>
+      <c r="B138" s="1" t="inlineStr">
+        <is>
+          <t>Total Quantity</t>
+        </is>
+      </c>
+      <c r="C138" s="1" t="inlineStr">
+        <is>
+          <t>Total Price</t>
+        </is>
       </c>
     </row>
     <row r="139">
-      <c r="H139" s="1" t="inlineStr">
-        <is>
-          <t>RUNNING GRAND TOTAL</t>
-        </is>
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>E2-0052</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>2</v>
+      </c>
+      <c r="C139" s="2" t="n">
+        <v>1.62</v>
       </c>
     </row>
     <row r="140">
-      <c r="H140" s="2" t="n">
-        <v>433.6289791666668</v>
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>E1-0199</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>6</v>
+      </c>
+      <c r="C140" s="2" t="n">
+        <v>19.44</v>
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="inlineStr">
-        <is>
-          <t>Part Number / Description</t>
-        </is>
-      </c>
-      <c r="B141" s="1" t="inlineStr">
-        <is>
-          <t>Total Quantity</t>
-        </is>
-      </c>
-      <c r="C141" s="1" t="inlineStr">
-        <is>
-          <t>Total Price</t>
-        </is>
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>E2-0047</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>6</v>
+      </c>
+      <c r="C141" s="2" t="n">
+        <v>14.28</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>E2-0052</t>
+          <t>PC-1220</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>2.666666666666667</v>
+        <v>24</v>
       </c>
       <c r="C142" s="2" t="n">
-        <v>2.16</v>
+        <v>4.391999999999999</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>E1-0199</t>
+          <t>PM-1006-SS</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C143" s="2" t="n">
-        <v>25.92</v>
+        <v>4.1985</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>E2-0047</t>
+          <t>UA-1212</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C144" s="2" t="n">
-        <v>19.04</v>
+        <v>5.832</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>PC-1220</t>
+          <t>E1-2530</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C145" s="2" t="n">
-        <v>5.856</v>
+        <v>27</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>PM-1006-SS</t>
+          <t>E2-0166</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C146" s="2" t="n">
-        <v>5.598</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>UA-1212</t>
+          <t>E2-0177</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C147" s="2" t="n">
-        <v>7.776</v>
+        <v>9.234000000000002</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>E1-2530</t>
+          <t>E2-0545</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C148" s="2" t="n">
-        <v>36</v>
+        <v>17.64</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>E2-0166</t>
+          <t>E2-0154</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -3320,33 +3310,33 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>E2-0177</t>
+          <t>E2-0611</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C150" s="2" t="n">
-        <v>12.312</v>
+        <v>11.43</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>E2-0545</t>
+          <t>BE9-2513</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>8</v>
+        <v>0.75</v>
       </c>
       <c r="C151" s="2" t="n">
-        <v>23.52</v>
+        <v>13.09375</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>E2-0154</t>
+          <t>E9-2512</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -3359,144 +3349,105 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>E2-0611</t>
+          <t>BE9-2511</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C153" s="2" t="n">
-        <v>15.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>BE9-2513</t>
+          <t>BE9-2515</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="C154" s="2" t="n">
-        <v>17.45833333333333</v>
+        <v>5.489583333333333</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>E9-2512</t>
+          <t>BE9-2514</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C155" s="2" t="n">
-        <v>0</v>
+        <v>4.625</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>BE9-2511</t>
+          <t>BE9-2578</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C156" s="2" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>BE9-2515</t>
+          <t>E9-2519</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.25</v>
       </c>
       <c r="C157" s="2" t="n">
-        <v>7.319444444444444</v>
+        <v>0.8859374999999999</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>BE9-2514</t>
+          <t>Glass Area</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1875</v>
       </c>
       <c r="C158" s="2" t="n">
-        <v>6.166666666666666</v>
+        <v>1.96875</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>BE9-2578</t>
+          <t>Joints Fabrication Labor</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.3333333333333333</v>
+        <v>12</v>
       </c>
       <c r="C159" s="2" t="n">
-        <v>3.666666666666667</v>
+        <v>180</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>E9-2519</t>
+          <t>Door size exceeds total glass area</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="C160" s="2" t="n">
-        <v>1.18125</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>Glass Area</t>
-        </is>
-      </c>
-      <c r="B161" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C161" s="2" t="n">
-        <v>2.625</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>Door size exceeds total glass area</t>
-        </is>
-      </c>
-      <c r="B162" t="n">
         <v>0</v>
-      </c>
-      <c r="C162" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>Joints Fabrication Labor</t>
-        </is>
-      </c>
-      <c r="B163" t="n">
-        <v>16</v>
-      </c>
-      <c r="C163" s="2" t="n">
-        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rought Draft For Optimization
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,13 +428,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
-    <col width="2" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
     <col width="2" customWidth="1" min="4" max="4"/>
     <col width="78" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
-    <col width="24" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -508,11 +508,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.16666666666666666 ft</t>
+          <t>16.0 ft</t>
         </is>
       </c>
       <c r="H3" s="2" t="n">
-        <v>2.909722222222222</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -536,11 +536,11 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.08333333333333333 ft</t>
+          <t>12.0 ft</t>
         </is>
       </c>
       <c r="H4" s="2" t="n">
-        <v>1.454861111111111</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -564,11 +564,11 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.0 ft</t>
+          <t>24.0 ft</t>
         </is>
       </c>
       <c r="H5" s="2" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -592,11 +592,11 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.0 ft</t>
+          <t>24.0 ft</t>
         </is>
       </c>
       <c r="H6" s="2" t="n">
-        <v>0</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -620,11 +620,11 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.08333333333333333 ft</t>
+          <t>12.0 ft</t>
         </is>
       </c>
       <c r="H7" s="2" t="n">
-        <v>1.829861111111111</v>
+        <v>527</v>
       </c>
     </row>
     <row r="8">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.006944444444444444</v>
+        <v>96</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -648,11 +648,11 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.08333333333333333 ft</t>
+          <t>12.0 ft</t>
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>1.541666666666667</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.006944444444444444</v>
+        <v>96</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -676,11 +676,11 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.08333333333333333 ft</t>
+          <t>12.0 ft</t>
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>0.9166666666666666</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3333333333333333</v>
+        <v>40</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -704,11 +704,11 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.08333333333333333 ft</t>
+          <t>24.0 ft</t>
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.2953125</v>
+        <v>85.05</v>
       </c>
     </row>
     <row r="11">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3333333333333333</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -753,241 +753,241 @@
     <row r="14">
       <c r="E14" t="inlineStr">
         <is>
-          <t>Glazing Gasket For 1” Glazing</t>
+          <t>End Dam For Sill Flashing</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>E2-0052</t>
+          <t>E1-0199</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.6666666666666666 ft</t>
+          <t>2 pcs</t>
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>0.54</v>
+        <v>64.8</v>
       </c>
     </row>
     <row r="15">
       <c r="E15" t="inlineStr">
         <is>
-          <t>End Dam For Sill Flashing</t>
+          <t>Water Deflector</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>E1-0199</t>
+          <t>E2-0047</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>8 pcs</t>
         </is>
       </c>
       <c r="H15" s="2" t="n">
-        <v>6.48</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16">
       <c r="E16" t="inlineStr">
         <is>
-          <t>Water Deflector</t>
+          <t>#12 x 1-1/4” PHSMS Type AB, Zinc Plated Steel, For Screw Spline Attachment</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>E2-0047</t>
+          <t>PC-1220</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>56 pcs</t>
         </is>
       </c>
       <c r="H16" s="2" t="n">
-        <v>4.76</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="17">
       <c r="E17" t="inlineStr">
         <is>
-          <t>#12 x 1-1/4” PHSMS Type AB, Zinc Plated Steel, For Screw Spline Attachment</t>
+          <t>#10-24 x 3/8” PHMS, Stainless Steel, For Attachment of Sill to Sill Flashing</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>PC-1220</t>
+          <t>PM-1006-SS</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>8 pcs</t>
+          <t>12 pcs</t>
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>1.464</v>
+        <v>46.65</v>
       </c>
     </row>
     <row r="18">
       <c r="E18" t="inlineStr">
         <is>
-          <t>#10-24 x 3/8” PHMS, Stainless Steel, For Attachment of Sill to Sill Flashing</t>
+          <t>#12 x 3/4” UFHSMS Type A, Zinc Plated Steel For End Dam Attachment</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>PM-1006-SS</t>
+          <t>UA-1212</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3 pcs</t>
+          <t>4 pcs</t>
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>1.3995</v>
+        <v>48.6</v>
       </c>
     </row>
     <row r="19">
       <c r="E19" t="inlineStr">
         <is>
-          <t>#12 x 3/4” UFHSMS Type A, Zinc Plated Steel For End Dam Attachment</t>
+          <t>Setting Block Chair Use with E2-0177 Setting Block at Sill</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>UA-1212</t>
+          <t>E1-2530</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>4 pcs</t>
+          <t>8 pcs</t>
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>1.944</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="E20" t="inlineStr">
         <is>
-          <t>Setting Block Chair Use with E2-0177 Setting Block at Sill</t>
+          <t>Side Block For Intermediate Vertical Shallow Pocket</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>E1-2530</t>
+          <t>E2-0166</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>6 pcs</t>
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>9</v>
+        <v>76.95</v>
       </c>
     </row>
     <row r="21">
       <c r="E21" t="inlineStr">
         <is>
-          <t>Side Block For Intermediate Vertical Shallow Pocket</t>
+          <t>Setting Block For Sill</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>E2-0166</t>
+          <t>E2-0177</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0 pcs</t>
+          <t>8 pcs</t>
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>0</v>
+        <v>76.95</v>
       </c>
     </row>
     <row r="22">
       <c r="E22" t="inlineStr">
         <is>
-          <t>Setting Block For Sill</t>
+          <t>1-1/8” “W” Side Block For Jamb</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>E2-0177</t>
+          <t>E2-0545</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>4 pcs</t>
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>3.078</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23">
       <c r="E23" t="inlineStr">
         <is>
-          <t>1-1/8” “W” Side Block For Jamb</t>
+          <t>1/2” “W” Side Block For Intermediate Vertical Deep Pocket</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>E2-0545</t>
+          <t>E2-0154</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>6 pcs</t>
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>5.88</v>
+        <v>56.7</v>
       </c>
     </row>
     <row r="24">
       <c r="E24" t="inlineStr">
         <is>
-          <t>1/2” “W” Side Block For Intermediate Vertical Deep Pocket</t>
+          <t>Setting Block For Intermediate Horizontal</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>E2-0154</t>
+          <t>E2-0611</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0 pcs</t>
+          <t>8 pcs</t>
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>0</v>
+        <v>95.25</v>
       </c>
     </row>
     <row r="25">
       <c r="E25" t="inlineStr">
         <is>
-          <t>Setting Block For Intermediate Horizontal</t>
+          <t>Gasket</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>E2-0611</t>
+          <t>E2-0052</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2 pcs</t>
+          <t>224.0 pcs</t>
         </is>
       </c>
       <c r="H25" s="2" t="n">
-        <v>3.81</v>
+        <v>90720</v>
       </c>
     </row>
     <row r="26">
@@ -1032,11 +1032,11 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0.0625 sqft</t>
+          <t>83.75 sqft</t>
         </is>
       </c>
       <c r="H28" s="2" t="n">
-        <v>0.65625</v>
+        <v>879.375</v>
       </c>
     </row>
     <row r="29">
@@ -1081,11 +1081,11 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>4 joints</t>
+          <t>24 joints</t>
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>60</v>
+        <v>360</v>
       </c>
     </row>
     <row r="32">
@@ -1097,19 +1097,971 @@
     </row>
     <row r="33">
       <c r="H33" s="2" t="n">
-        <v>107.9598402777778</v>
+        <v>95550.625</v>
       </c>
     </row>
     <row r="34">
-      <c r="H34" s="1" t="inlineStr">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>System Input</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>YES 45TU FRONT SET(OG)</t>
+        </is>
+      </c>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>PROFILES</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Elevation Type</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G35" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H35" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Total Count</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Sill/Jamb Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>16.0 ft</t>
+        </is>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t># Bays Wide</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>4</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Sill/Jamb Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>12.0 ft</t>
+        </is>
+      </c>
+      <c r="H37" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t># Bays Tall</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Flush Filler</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>E9-2512</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>24.0 ft</t>
+        </is>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Opening Width</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>144</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Two Piece Mullion Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>BE9-2511</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>24.0 ft</t>
+        </is>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Opening Height</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>96</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Horizontal Screw Spline Assembly</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>BE9-2515</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>12.0 ft</t>
+        </is>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>Sq Ft per Type</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>96</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Head</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>BE9-2514</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>12.0 ft</t>
+        </is>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>Total Sq Ft</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>96</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Thermal Sill Flashing</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>BE9-2578</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>12.0 ft</t>
+        </is>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>Perimeter Ft</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>40</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Glass Stop (Use with BE9-2514, BE9-2515, BE9-2517)</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>E9-2519</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>24.0 ft</t>
+        </is>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>85.05</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>Total Perimeter Ft</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>ACCESSORIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G46" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H46" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>End Dam For Sill Flashing</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>E1-0199</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2 pcs</t>
+        </is>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Water Deflector</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>E2-0047</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>#12 x 1-1/4” PHSMS Type AB, Zinc Plated Steel, For Screw Spline Attachment</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>PC-1220</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>56 pcs</t>
+        </is>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>#10-24 x 3/8” PHMS, Stainless Steel, For Attachment of Sill to Sill Flashing</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>PM-1006-SS</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>12 pcs</t>
+        </is>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>#12 x 3/4” UFHSMS Type A, Zinc Plated Steel For End Dam Attachment</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>UA-1212</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>4 pcs</t>
+        </is>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Setting Block Chair Use with E2-0177 Setting Block at Sill</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>E1-2530</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Side Block For Intermediate Vertical Shallow Pocket</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>E2-0166</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>6 pcs</t>
+        </is>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Setting Block For Sill</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>E2-0177</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>1-1/8” “W” Side Block For Jamb</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>E2-0545</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>4 pcs</t>
+        </is>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>1/2” “W” Side Block For Intermediate Vertical Deep Pocket</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>E2-0154</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>6 pcs</t>
+        </is>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Setting Block For Intermediate Horizontal</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>E2-0611</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>8 pcs</t>
+        </is>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Gasket</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>E2-0052</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>224.0 pcs</t>
+        </is>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>90720</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="E59" s="1" t="inlineStr">
+        <is>
+          <t>GLASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F60" s="1" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G60" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H60" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Glass Area</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>83.75 sqft</t>
+        </is>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>879.375</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="E62" s="1" t="inlineStr">
+        <is>
+          <t>FABRICATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="E63" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F63" s="1" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="G63" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H63" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Joints Fabrication Labor</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>24 joints</t>
+        </is>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="H65" s="1" t="inlineStr">
+        <is>
+          <t>SYSTEM TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="H66" s="2" t="n">
+        <v>93164.72500000001</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="H67" s="1" t="inlineStr">
         <is>
           <t>RUNNING GRAND TOTAL</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="H35" s="2" t="n">
-        <v>107.9598402777778</v>
+    <row r="68">
+      <c r="H68" s="2" t="n">
+        <v>188715.35</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>Part Number / Description</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>Total Quantity</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>Total Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>E1-0199</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>4</v>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>E2-0047</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>16</v>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>PC-1220</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>112</v>
+      </c>
+      <c r="C72" s="2" t="n">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>PM-1006-SS</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>24</v>
+      </c>
+      <c r="C73" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>UA-1212</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>8</v>
+      </c>
+      <c r="C74" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>E1-2530</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>16</v>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>E2-0166</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>12</v>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>E2-0177</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>16</v>
+      </c>
+      <c r="C77" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>E2-0545</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>8</v>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>E2-0154</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>12</v>
+      </c>
+      <c r="C79" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>E2-0611</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>16</v>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>BE9-2513</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>56</v>
+      </c>
+      <c r="C81" s="2" t="n">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>E9-2512</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>48</v>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>BE9-2511</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>48</v>
+      </c>
+      <c r="C83" s="2" t="n">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>BE9-2515</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>24</v>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>BE9-2514</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>24</v>
+      </c>
+      <c r="C85" s="2" t="n">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>BE9-2578</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>24</v>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>E9-2519</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>48</v>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>170.1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Glass Area</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>167.5</v>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>1758.75</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Joints Fabrication Labor</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>48</v>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>E2-0052</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>448</v>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>181440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>